<commit_message>
Full rebuild of project
Add input to all sorts, rebuild input: change input by hands for define
constants. Remove MergeSort from result list
</commit_message>
<xml_diff>
--- a/Книга1.xlsx
+++ b/Книга1.xlsx
@@ -30,9 +30,6 @@
     <t>Quick</t>
   </si>
   <si>
-    <t>Merge</t>
-  </si>
-  <si>
     <t>Random input</t>
   </si>
   <si>
@@ -44,13 +41,16 @@
   <si>
     <t>Execution Time</t>
   </si>
+  <si>
+    <t>89.393</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -88,7 +88,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -258,51 +258,6 @@
       <top style="thin">
         <color auto="1"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -310,19 +265,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -332,18 +287,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -645,10 +597,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:S15"/>
+  <dimension ref="A2:S14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -657,56 +609,56 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="5"/>
-      <c r="S2" s="12"/>
+      <c r="B2" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="14"/>
+      <c r="P2" s="14"/>
+      <c r="Q2" s="14"/>
+      <c r="R2" s="14"/>
+      <c r="S2" s="15"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="6" t="s">
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="12"/>
+      <c r="N3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="O3" s="7"/>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="7"/>
-      <c r="R3" s="7"/>
-      <c r="S3" s="8"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="11"/>
+      <c r="S3" s="12"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
-      <c r="B4" s="9">
+      <c r="B4" s="4">
         <v>100</v>
       </c>
       <c r="C4" s="1">
@@ -721,10 +673,10 @@
       <c r="F4" s="1">
         <v>50000</v>
       </c>
-      <c r="G4" s="10">
+      <c r="G4" s="5">
         <v>100000</v>
       </c>
-      <c r="H4" s="11">
+      <c r="H4" s="6">
         <v>100</v>
       </c>
       <c r="I4" s="1">
@@ -739,10 +691,10 @@
       <c r="L4" s="1">
         <v>50000</v>
       </c>
-      <c r="M4" s="10">
+      <c r="M4" s="5">
         <v>100000</v>
       </c>
-      <c r="N4" s="11">
+      <c r="N4" s="6">
         <v>100</v>
       </c>
       <c r="O4" s="1">
@@ -757,7 +709,7 @@
       <c r="R4" s="1">
         <v>50000</v>
       </c>
-      <c r="S4" s="10">
+      <c r="S4" s="5">
         <v>100000</v>
       </c>
     </row>
@@ -765,124 +717,117 @@
       <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="13">
-        <v>7.1849999999999996</v>
-      </c>
-      <c r="C5" s="14">
-        <v>14.009</v>
-      </c>
-      <c r="D5" s="14">
-        <v>10.829000000000001</v>
-      </c>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14"/>
-      <c r="M5" s="15"/>
-      <c r="N5" s="13"/>
-      <c r="O5" s="14"/>
-      <c r="P5" s="14"/>
-      <c r="Q5" s="14"/>
-      <c r="R5" s="14"/>
-      <c r="S5" s="15"/>
+      <c r="B5" s="7">
+        <v>4.5860000000000003</v>
+      </c>
+      <c r="C5" s="8">
+        <v>7.875</v>
+      </c>
+      <c r="D5" s="8">
+        <v>9.875</v>
+      </c>
+      <c r="E5" s="8">
+        <v>14.28</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="9">
+        <v>207.75</v>
+      </c>
+      <c r="H5" s="7">
+        <v>4.1269999999999998</v>
+      </c>
+      <c r="I5" s="8">
+        <v>6.7629999999999999</v>
+      </c>
+      <c r="J5" s="8">
+        <v>9.3810000000000002</v>
+      </c>
+      <c r="K5" s="8">
+        <v>10.225</v>
+      </c>
+      <c r="L5" s="8"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="7">
+        <v>5.0229999999999997</v>
+      </c>
+      <c r="O5" s="8"/>
+      <c r="P5" s="8"/>
+      <c r="Q5" s="8"/>
+      <c r="R5" s="8"/>
+      <c r="S5" s="9"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="15"/>
-      <c r="N6" s="13"/>
-      <c r="O6" s="14"/>
-      <c r="P6" s="14"/>
-      <c r="Q6" s="14"/>
-      <c r="R6" s="14"/>
-      <c r="S6" s="15"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="8"/>
+      <c r="P6" s="8"/>
+      <c r="Q6" s="8"/>
+      <c r="R6" s="8"/>
+      <c r="S6" s="9"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="14"/>
-      <c r="M7" s="15"/>
-      <c r="N7" s="13"/>
-      <c r="O7" s="14"/>
-      <c r="P7" s="14"/>
-      <c r="Q7" s="14"/>
-      <c r="R7" s="14"/>
-      <c r="S7" s="15"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="8"/>
+      <c r="P7" s="8"/>
+      <c r="Q7" s="8"/>
+      <c r="R7" s="8"/>
+      <c r="S7" s="9"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="15"/>
-      <c r="N8" s="13"/>
-      <c r="O8" s="14"/>
-      <c r="P8" s="14"/>
-      <c r="Q8" s="14"/>
-      <c r="R8" s="14"/>
-      <c r="S8" s="15"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="8"/>
+      <c r="P8" s="8"/>
+      <c r="Q8" s="8"/>
+      <c r="R8" s="8"/>
+      <c r="S8" s="9"/>
     </row>
-    <row r="9" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="17"/>
-      <c r="K9" s="17"/>
-      <c r="L9" s="17"/>
-      <c r="M9" s="18"/>
-      <c r="N9" s="16"/>
-      <c r="O9" s="17"/>
-      <c r="P9" s="17"/>
-      <c r="Q9" s="17"/>
-      <c r="R9" s="17"/>
-      <c r="S9" s="18"/>
-    </row>
-    <row r="15" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="B3:G3"/>

</xml_diff>

<commit_message>
Complete to full up the result table
</commit_message>
<xml_diff>
--- a/Книга1.xlsx
+++ b/Книга1.xlsx
@@ -306,168 +306,6 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Лист1!$A$5</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Bubble</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:multiLvlStrRef>
-              <c:f>Лист1!$B$2:$S$4</c:f>
-              <c:multiLvlStrCache>
-                <c:ptCount val="18"/>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>100</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>1000</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>5000</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>10000</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>50000</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>100000</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>100</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>1000</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>5000</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>10000</c:v>
-                  </c:pt>
-                  <c:pt idx="10">
-                    <c:v>50000</c:v>
-                  </c:pt>
-                  <c:pt idx="11">
-                    <c:v>100000</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>100</c:v>
-                  </c:pt>
-                  <c:pt idx="13">
-                    <c:v>1000</c:v>
-                  </c:pt>
-                  <c:pt idx="14">
-                    <c:v>5000</c:v>
-                  </c:pt>
-                  <c:pt idx="15">
-                    <c:v>10000</c:v>
-                  </c:pt>
-                  <c:pt idx="16">
-                    <c:v>50000</c:v>
-                  </c:pt>
-                  <c:pt idx="17">
-                    <c:v>100000</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Random input</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>Best input</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>Worst input</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Execution Time</c:v>
-                  </c:pt>
-                </c:lvl>
-              </c:multiLvlStrCache>
-            </c:multiLvlStrRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Лист1!$B$5:$S$5</c:f>
-              <c:numCache>
-                <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="18"/>
-                <c:pt idx="0">
-                  <c:v>1.9530000000000001</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.734</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.0629999999999997</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5.1040000000000001</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>45.26</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>147.517</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.47299999999999998</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.4690000000000001</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3.214</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>5.09</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>15.266</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>30.23</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>2.5310000000000001</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1.6879999999999999</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>3.181</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>5.9219999999999997</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>48.085000000000001</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>160.04</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
@@ -482,229 +320,7 @@
             </c:strRef>
           </c:tx>
           <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:multiLvlStrRef>
-              <c:f>Лист1!$B$2:$S$4</c:f>
-              <c:multiLvlStrCache>
-                <c:ptCount val="18"/>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>100</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>1000</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>5000</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>10000</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>50000</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>100000</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>100</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>1000</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>5000</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>10000</c:v>
-                  </c:pt>
-                  <c:pt idx="10">
-                    <c:v>50000</c:v>
-                  </c:pt>
-                  <c:pt idx="11">
-                    <c:v>100000</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>100</c:v>
-                  </c:pt>
-                  <c:pt idx="13">
-                    <c:v>1000</c:v>
-                  </c:pt>
-                  <c:pt idx="14">
-                    <c:v>5000</c:v>
-                  </c:pt>
-                  <c:pt idx="15">
-                    <c:v>10000</c:v>
-                  </c:pt>
-                  <c:pt idx="16">
-                    <c:v>50000</c:v>
-                  </c:pt>
-                  <c:pt idx="17">
-                    <c:v>100000</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Random input</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>Best input</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>Worst input</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Execution Time</c:v>
-                  </c:pt>
-                </c:lvl>
-              </c:multiLvlStrCache>
-            </c:multiLvlStrRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Лист1!$B$6:$S$6</c:f>
-              <c:numCache>
-                <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="18"/>
-                <c:pt idx="0">
-                  <c:v>1.141</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.40600000000000003</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Лист1!$A$7</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Shell</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:multiLvlStrRef>
-              <c:f>Лист1!$B$2:$S$4</c:f>
-              <c:multiLvlStrCache>
-                <c:ptCount val="18"/>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>100</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>1000</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>5000</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>10000</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>50000</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>100000</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>100</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>1000</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>5000</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>10000</c:v>
-                  </c:pt>
-                  <c:pt idx="10">
-                    <c:v>50000</c:v>
-                  </c:pt>
-                  <c:pt idx="11">
-                    <c:v>100000</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>100</c:v>
-                  </c:pt>
-                  <c:pt idx="13">
-                    <c:v>1000</c:v>
-                  </c:pt>
-                  <c:pt idx="14">
-                    <c:v>5000</c:v>
-                  </c:pt>
-                  <c:pt idx="15">
-                    <c:v>10000</c:v>
-                  </c:pt>
-                  <c:pt idx="16">
-                    <c:v>50000</c:v>
-                  </c:pt>
-                  <c:pt idx="17">
-                    <c:v>100000</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Random input</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>Best input</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>Worst input</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Execution Time</c:v>
-                  </c:pt>
-                </c:lvl>
-              </c:multiLvlStrCache>
-            </c:multiLvlStrRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Лист1!$B$7:$S$7</c:f>
-              <c:numCache>
-                <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="18"/>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Лист1!$A$8</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Quick</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="square"/>
+            <c:symbol val="circle"/>
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
@@ -803,6 +419,362 @@
           </c:cat>
           <c:val>
             <c:numRef>
+              <c:f>Лист1!$B$6:$S$6</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>1.1419999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.859</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0940000000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.0229999999999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>27.143999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>67.001000000000005</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.5720000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.0630000000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.008</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.9930000000000003</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>20.530999999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.125</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.7809999999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4.4370000000000003</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5.609</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>34.826999999999998</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>93.14</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Shell</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLblPos val="l"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Лист1!$B$2:$S$4</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="18"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>100</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1000</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>5000</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>10000</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>50000</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>100000</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>100</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>1000</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>5000</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>10000</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>50000</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>100000</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>100</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>1000</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>5000</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>10000</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>50000</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>100000</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Random input</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Best input</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>Worst input</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Execution Time</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$B$7:$S$7</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>2.609</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.875</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.1879999999999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>21.015999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>39.438000000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.069</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.875</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.7810000000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.8280000000000003</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>20.734000000000002</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>38.671999999999997</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.359</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.9060000000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.948</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5.0469999999999997</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>21.484000000000002</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>40.398000000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Quick</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="4"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Лист1!$B$2:$S$4</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="18"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>100</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1000</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>5000</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>10000</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>50000</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>100000</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>100</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>1000</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>5000</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>10000</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>50000</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>100000</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>100</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>1000</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>5000</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>10000</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>50000</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>100000</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Random input</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Best input</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>Worst input</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Execution Time</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
               <c:f>Лист1!$B$8:$S$8</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
@@ -876,20 +848,216 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="73405952"/>
-        <c:axId val="73407488"/>
+        <c:axId val="114606848"/>
+        <c:axId val="114608384"/>
+      </c:lineChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Bubble</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Лист1!$B$2:$S$4</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="18"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>100</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1000</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>5000</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>10000</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>50000</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>100000</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>100</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>1000</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>5000</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>10000</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>50000</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>100000</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>100</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>1000</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>5000</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>10000</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>50000</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>100000</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Random input</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Best input</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>Worst input</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Execution Time</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$B$5:$S$5</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>1.9530000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.734</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0629999999999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.1040000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45.26</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>147.517</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.47299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.4690000000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.214</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.09</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>15.266</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>30.23</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.5310000000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.6879999999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.181</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5.9219999999999997</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>48.085000000000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>160.04</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="120342016"/>
+        <c:axId val="103373824"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="73405952"/>
+        <c:axId val="114606848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73407488"/>
+        <c:crossAx val="114608384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -897,7 +1065,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="73407488"/>
+        <c:axId val="114608384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -908,10 +1076,41 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73405952"/>
+        <c:crossAx val="114606848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
+      <c:valAx>
+        <c:axId val="103373824"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="120342016"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="120342016"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="103373824"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
       <c:spPr>
         <a:ln>
           <a:solidFill>
@@ -948,16 +1147,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>0</xdr:col>
       <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>523875</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>600074</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1269,7 +1468,7 @@
   <dimension ref="A2:S14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="T10" sqref="T10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1446,50 +1645,118 @@
         <v>1</v>
       </c>
       <c r="B6" s="7">
-        <v>1.141</v>
+        <v>1.1419999999999999</v>
       </c>
       <c r="C6" s="7">
-        <v>0.40600000000000003</v>
-      </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
-      <c r="N6" s="7"/>
-      <c r="O6" s="7"/>
-      <c r="P6" s="7"/>
-      <c r="Q6" s="7"/>
-      <c r="R6" s="7"/>
-      <c r="S6" s="7"/>
+        <v>1.859</v>
+      </c>
+      <c r="D6" s="7">
+        <v>4.0940000000000003</v>
+      </c>
+      <c r="E6" s="7">
+        <v>6.0229999999999997</v>
+      </c>
+      <c r="F6" s="7">
+        <v>27.143999999999998</v>
+      </c>
+      <c r="G6" s="7">
+        <v>67.001000000000005</v>
+      </c>
+      <c r="H6" s="7">
+        <v>1.5720000000000001</v>
+      </c>
+      <c r="I6" s="7">
+        <v>2.0630000000000002</v>
+      </c>
+      <c r="J6" s="7">
+        <v>3.008</v>
+      </c>
+      <c r="K6" s="7">
+        <v>5.9930000000000003</v>
+      </c>
+      <c r="L6" s="7">
+        <v>20.530999999999999</v>
+      </c>
+      <c r="M6" s="7">
+        <v>40</v>
+      </c>
+      <c r="N6" s="7">
+        <v>2.125</v>
+      </c>
+      <c r="O6" s="7">
+        <v>1.7809999999999999</v>
+      </c>
+      <c r="P6" s="7">
+        <v>4.4370000000000003</v>
+      </c>
+      <c r="Q6" s="7">
+        <v>5.609</v>
+      </c>
+      <c r="R6" s="7">
+        <v>34.826999999999998</v>
+      </c>
+      <c r="S6" s="7">
+        <v>93.14</v>
+      </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="7"/>
-      <c r="Q7" s="7"/>
-      <c r="R7" s="7"/>
-      <c r="S7" s="7"/>
+      <c r="B7" s="7">
+        <v>2.609</v>
+      </c>
+      <c r="C7" s="7">
+        <v>2.875</v>
+      </c>
+      <c r="D7" s="7">
+        <v>3.75</v>
+      </c>
+      <c r="E7" s="7">
+        <v>6.1879999999999997</v>
+      </c>
+      <c r="F7" s="7">
+        <v>21.015999999999998</v>
+      </c>
+      <c r="G7" s="7">
+        <v>39.438000000000002</v>
+      </c>
+      <c r="H7" s="7">
+        <v>2.069</v>
+      </c>
+      <c r="I7" s="7">
+        <v>2.875</v>
+      </c>
+      <c r="J7" s="7">
+        <v>3.7810000000000001</v>
+      </c>
+      <c r="K7" s="7">
+        <v>4.8280000000000003</v>
+      </c>
+      <c r="L7" s="7">
+        <v>20.734000000000002</v>
+      </c>
+      <c r="M7" s="7">
+        <v>38.671999999999997</v>
+      </c>
+      <c r="N7" s="7">
+        <v>2.359</v>
+      </c>
+      <c r="O7" s="7">
+        <v>2.9060000000000001</v>
+      </c>
+      <c r="P7" s="7">
+        <v>3.948</v>
+      </c>
+      <c r="Q7" s="7">
+        <v>5.0469999999999997</v>
+      </c>
+      <c r="R7" s="7">
+        <v>21.484000000000002</v>
+      </c>
+      <c r="S7" s="7">
+        <v>40.398000000000003</v>
+      </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">

</xml_diff>

<commit_message>
Add the new sheet in excel table wth result
Wth result in numbers of transpositions and comparings
</commit_message>
<xml_diff>
--- a/Книга1.xlsx
+++ b/Книга1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="20730" windowHeight="11760" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="10">
   <si>
     <t>Bubble</t>
   </si>
@@ -40,6 +40,12 @@
   </si>
   <si>
     <t>Execution Time</t>
+  </si>
+  <si>
+    <t>Number Of Comparings</t>
+  </si>
+  <si>
+    <t>Number Of Transpositions</t>
   </si>
 </sst>
 </file>
@@ -232,7 +238,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -261,6 +267,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -848,8 +855,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="114606848"/>
-        <c:axId val="114608384"/>
+        <c:axId val="50624000"/>
+        <c:axId val="50625536"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1043,11 +1050,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="120342016"/>
-        <c:axId val="103373824"/>
+        <c:axId val="50632960"/>
+        <c:axId val="50631424"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="114606848"/>
+        <c:axId val="50624000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1057,7 +1064,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="114608384"/>
+        <c:crossAx val="50625536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1065,7 +1072,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="114608384"/>
+        <c:axId val="50625536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1076,12 +1083,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="114606848"/>
+        <c:crossAx val="50624000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="103373824"/>
+        <c:axId val="50631424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1091,12 +1098,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="120342016"/>
+        <c:crossAx val="50632960"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="120342016"/>
+        <c:axId val="50632960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1105,7 +1112,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103373824"/>
+        <c:crossAx val="50631424"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -1143,6 +1151,1310 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист2!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Bubble</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Лист2!$B$1:$Q$3</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="15"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>100</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1000</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>5000</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>10000</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>50000</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>100</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>1000</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>5000</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>10000</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>50000</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>100</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>1000</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>5000</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>10000</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>50000</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Random input</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Best input</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>Worst input</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Number Of Comparings</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист2!$B$4:$Q$4</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>2372</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>247855</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6301027</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25186062</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>625822298</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>344</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>344</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>344</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>344</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4851</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>498947</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12492947</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>49985447</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1249925447</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист2!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Insertion</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Лист2!$B$1:$Q$3</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="15"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>100</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1000</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>5000</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>10000</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>50000</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>100</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>1000</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>5000</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>10000</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>50000</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>100</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>1000</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>5000</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>10000</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>50000</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Random input</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Best input</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>Worst input</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Number Of Comparings</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист2!$B$5:$Q$5</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>2501</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>250364</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6263870</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24742388</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>622195734</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>196</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1343</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5343</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10343</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50343</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4852</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>499500</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12497500</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>49995000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1249975000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист2!$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Shell</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Лист2!$B$1:$Q$3</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="15"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>100</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1000</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>5000</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>10000</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>50000</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>100</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>1000</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>5000</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>10000</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>50000</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>100</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>1000</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>5000</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>10000</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>50000</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Random input</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Best input</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>Worst input</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Number Of Comparings</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист2!$B$6:$Q$6</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>940</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14852</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>112646</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>257359</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1806986</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>595</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8434</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>55342</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>120342</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>700343</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>744</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11735</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>78143</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>171212</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1018691</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист2!$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Quick</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Лист2!$B$1:$Q$3</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="15"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>100</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1000</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>5000</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>10000</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>50000</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>100</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>1000</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>5000</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>10000</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>50000</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>100</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>1000</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>5000</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>10000</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>50000</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Random input</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Best input</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>Worst input</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Number Of Comparings</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист2!$B$7:$Q$7</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>532</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8213</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>48893</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>116593</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>645555</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>578</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9631</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>61464</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>133272</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>784119</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>575</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8730</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>56563</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>123371</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>754217</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="69360640"/>
+        <c:axId val="69608192"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="69360640"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="69608192"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="69608192"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="69360640"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:dispUnits>
+          <c:builtInUnit val="thousands"/>
+          <c:dispUnitsLbl>
+            <c:layout/>
+          </c:dispUnitsLbl>
+        </c:dispUnits>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист2!$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Bubble</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Лист2!$B$9:$P$11</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="15"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>100</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1000</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>5000</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>10000</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>50000</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>100</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>1000</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>5000</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>10000</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>50000</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>100</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>1000</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>5000</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>10000</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>50000</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Random input</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Best input</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>Worst input</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Number Of Transpositions</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист2!$B$12:$P$12</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>2372</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>247855</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6301027</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25186062</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>625822298</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>344</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>344</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>344</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>344</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4851</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>498947</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12492947</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>49985447</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1249925447</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист2!$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Insertion</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Лист2!$B$9:$P$11</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="15"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>100</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1000</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>5000</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>10000</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>50000</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>100</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>1000</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>5000</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>10000</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>50000</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>100</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>1000</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>5000</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>10000</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>50000</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Random input</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Best input</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>Worst input</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Number Of Transpositions</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист2!$B$13:$P$13</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>2405</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>249373</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6258876</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24732396</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>622145750</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>344</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>344</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>344</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>344</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4851</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>498947</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12492947</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>49985447</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1249925447</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист2!$A$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Shell</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Лист2!$B$9:$P$11</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="15"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>100</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1000</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>5000</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>10000</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>50000</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>100</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>1000</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>5000</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>10000</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>50000</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>100</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>1000</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>5000</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>10000</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>50000</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Random input</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Best input</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>Worst input</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Number Of Transpositions</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист2!$B$14:$P$14</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>487</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7369</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>60182</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1422475</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1132440</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>344</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>343</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>344</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>344</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>373</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4718</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>28122</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>61190</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>368660</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист2!$A$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Quick</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Лист2!$B$9:$P$11</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="15"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>100</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1000</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>5000</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>10000</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>50000</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>100</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>1000</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>5000</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>10000</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>50000</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>100</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>1000</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>5000</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>10000</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>50000</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Random input</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Best input</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>Worst input</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Number Of Transpositions</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист2!$B$15:$P$15</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>179</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2539</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15372</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>32481</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>194860</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>345</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>345</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>345</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>345</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>748</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2748</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5248</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>25248</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="89783296"/>
+        <c:axId val="90047232"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="89783296"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="90047232"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="90047232"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="89783296"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1170,6 +2482,71 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Диаграмма 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>361949</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>152399</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Диаграмма 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1467,8 +2844,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:S14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T10" sqref="T10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1833,13 +3210,612 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:P15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="P15" sqref="A9:P15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="9"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="4">
+        <v>100</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1000</v>
+      </c>
+      <c r="D3" s="1">
+        <v>5000</v>
+      </c>
+      <c r="E3" s="1">
+        <v>10000</v>
+      </c>
+      <c r="F3" s="1">
+        <v>50000</v>
+      </c>
+      <c r="G3" s="6">
+        <v>100</v>
+      </c>
+      <c r="H3" s="1">
+        <v>1000</v>
+      </c>
+      <c r="I3" s="1">
+        <v>5000</v>
+      </c>
+      <c r="J3" s="1">
+        <v>10000</v>
+      </c>
+      <c r="K3" s="1">
+        <v>50000</v>
+      </c>
+      <c r="L3" s="6">
+        <v>100</v>
+      </c>
+      <c r="M3" s="1">
+        <v>1000</v>
+      </c>
+      <c r="N3" s="1">
+        <v>5000</v>
+      </c>
+      <c r="O3" s="1">
+        <v>10000</v>
+      </c>
+      <c r="P3" s="1">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="14">
+        <v>2372</v>
+      </c>
+      <c r="C4" s="14">
+        <v>247855</v>
+      </c>
+      <c r="D4" s="14">
+        <v>6301027</v>
+      </c>
+      <c r="E4" s="14">
+        <v>25186062</v>
+      </c>
+      <c r="F4" s="14">
+        <v>625822298</v>
+      </c>
+      <c r="G4" s="14">
+        <v>97</v>
+      </c>
+      <c r="H4" s="14">
+        <v>344</v>
+      </c>
+      <c r="I4" s="14">
+        <v>344</v>
+      </c>
+      <c r="J4" s="14">
+        <v>344</v>
+      </c>
+      <c r="K4" s="14">
+        <v>344</v>
+      </c>
+      <c r="L4" s="14">
+        <v>4851</v>
+      </c>
+      <c r="M4" s="14">
+        <v>498947</v>
+      </c>
+      <c r="N4" s="14">
+        <v>12492947</v>
+      </c>
+      <c r="O4" s="14">
+        <v>49985447</v>
+      </c>
+      <c r="P4" s="14">
+        <v>1249925447</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="14">
+        <v>2501</v>
+      </c>
+      <c r="C5" s="14">
+        <v>250364</v>
+      </c>
+      <c r="D5" s="14">
+        <v>6263870</v>
+      </c>
+      <c r="E5" s="14">
+        <v>24742388</v>
+      </c>
+      <c r="F5" s="14">
+        <v>622195734</v>
+      </c>
+      <c r="G5" s="14">
+        <v>196</v>
+      </c>
+      <c r="H5" s="14">
+        <v>1343</v>
+      </c>
+      <c r="I5" s="14">
+        <v>5343</v>
+      </c>
+      <c r="J5" s="14">
+        <v>10343</v>
+      </c>
+      <c r="K5" s="14">
+        <v>50343</v>
+      </c>
+      <c r="L5" s="14">
+        <v>4852</v>
+      </c>
+      <c r="M5" s="14">
+        <v>499500</v>
+      </c>
+      <c r="N5" s="14">
+        <v>12497500</v>
+      </c>
+      <c r="O5" s="14">
+        <v>49995000</v>
+      </c>
+      <c r="P5" s="14">
+        <v>1249975000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="14">
+        <v>940</v>
+      </c>
+      <c r="C6" s="14">
+        <v>14852</v>
+      </c>
+      <c r="D6" s="14">
+        <v>112646</v>
+      </c>
+      <c r="E6" s="14">
+        <v>257359</v>
+      </c>
+      <c r="F6" s="14">
+        <v>1806986</v>
+      </c>
+      <c r="G6" s="14">
+        <v>595</v>
+      </c>
+      <c r="H6" s="14">
+        <v>8434</v>
+      </c>
+      <c r="I6" s="14">
+        <v>55342</v>
+      </c>
+      <c r="J6" s="14">
+        <v>120342</v>
+      </c>
+      <c r="K6" s="14">
+        <v>700343</v>
+      </c>
+      <c r="L6" s="14">
+        <v>744</v>
+      </c>
+      <c r="M6" s="14">
+        <v>11735</v>
+      </c>
+      <c r="N6" s="14">
+        <v>78143</v>
+      </c>
+      <c r="O6" s="14">
+        <v>171212</v>
+      </c>
+      <c r="P6" s="14">
+        <v>1018691</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="14">
+        <v>532</v>
+      </c>
+      <c r="C7" s="14">
+        <v>8213</v>
+      </c>
+      <c r="D7" s="14">
+        <v>48893</v>
+      </c>
+      <c r="E7" s="14">
+        <v>116593</v>
+      </c>
+      <c r="F7" s="14">
+        <v>645555</v>
+      </c>
+      <c r="G7" s="14">
+        <v>578</v>
+      </c>
+      <c r="H7" s="14">
+        <v>9631</v>
+      </c>
+      <c r="I7" s="14">
+        <v>61464</v>
+      </c>
+      <c r="J7" s="14">
+        <v>133272</v>
+      </c>
+      <c r="K7" s="14">
+        <v>784119</v>
+      </c>
+      <c r="L7" s="14">
+        <v>575</v>
+      </c>
+      <c r="M7" s="14">
+        <v>8730</v>
+      </c>
+      <c r="N7" s="14">
+        <v>56563</v>
+      </c>
+      <c r="O7" s="14">
+        <v>123371</v>
+      </c>
+      <c r="P7" s="14">
+        <v>754217</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="12"/>
+      <c r="N9" s="12"/>
+      <c r="O9" s="12"/>
+      <c r="P9" s="12"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B10" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
+      <c r="P10" s="9"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="4">
+        <v>100</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1000</v>
+      </c>
+      <c r="D11" s="1">
+        <v>5000</v>
+      </c>
+      <c r="E11" s="1">
+        <v>10000</v>
+      </c>
+      <c r="F11" s="1">
+        <v>50000</v>
+      </c>
+      <c r="G11" s="6">
+        <v>100</v>
+      </c>
+      <c r="H11" s="1">
+        <v>1000</v>
+      </c>
+      <c r="I11" s="1">
+        <v>5000</v>
+      </c>
+      <c r="J11" s="1">
+        <v>10000</v>
+      </c>
+      <c r="K11" s="1">
+        <v>50000</v>
+      </c>
+      <c r="L11" s="6">
+        <v>100</v>
+      </c>
+      <c r="M11" s="1">
+        <v>1000</v>
+      </c>
+      <c r="N11" s="1">
+        <v>5000</v>
+      </c>
+      <c r="O11" s="1">
+        <v>10000</v>
+      </c>
+      <c r="P11" s="1">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="14">
+        <v>2372</v>
+      </c>
+      <c r="C12" s="14">
+        <v>247855</v>
+      </c>
+      <c r="D12" s="14">
+        <v>6301027</v>
+      </c>
+      <c r="E12" s="14">
+        <v>25186062</v>
+      </c>
+      <c r="F12" s="14">
+        <v>625822298</v>
+      </c>
+      <c r="G12" s="14">
+        <v>97</v>
+      </c>
+      <c r="H12" s="14">
+        <v>344</v>
+      </c>
+      <c r="I12" s="14">
+        <v>344</v>
+      </c>
+      <c r="J12" s="14">
+        <v>344</v>
+      </c>
+      <c r="K12" s="14">
+        <v>344</v>
+      </c>
+      <c r="L12" s="14">
+        <v>4851</v>
+      </c>
+      <c r="M12" s="14">
+        <v>498947</v>
+      </c>
+      <c r="N12" s="14">
+        <v>12492947</v>
+      </c>
+      <c r="O12" s="14">
+        <v>49985447</v>
+      </c>
+      <c r="P12" s="14">
+        <v>1249925447</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="14">
+        <v>2405</v>
+      </c>
+      <c r="C13" s="14">
+        <v>249373</v>
+      </c>
+      <c r="D13" s="14">
+        <v>6258876</v>
+      </c>
+      <c r="E13" s="14">
+        <v>24732396</v>
+      </c>
+      <c r="F13" s="14">
+        <v>622145750</v>
+      </c>
+      <c r="G13" s="14">
+        <v>97</v>
+      </c>
+      <c r="H13" s="14">
+        <v>344</v>
+      </c>
+      <c r="I13" s="14">
+        <v>344</v>
+      </c>
+      <c r="J13" s="14">
+        <v>344</v>
+      </c>
+      <c r="K13" s="14">
+        <v>344</v>
+      </c>
+      <c r="L13" s="14">
+        <v>4851</v>
+      </c>
+      <c r="M13" s="14">
+        <v>498947</v>
+      </c>
+      <c r="N13" s="14">
+        <v>12492947</v>
+      </c>
+      <c r="O13" s="14">
+        <v>49985447</v>
+      </c>
+      <c r="P13" s="14">
+        <v>1249925447</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="14">
+        <v>487</v>
+      </c>
+      <c r="C14" s="14">
+        <v>7369</v>
+      </c>
+      <c r="D14" s="14">
+        <v>60182</v>
+      </c>
+      <c r="E14" s="14">
+        <v>1422475</v>
+      </c>
+      <c r="F14" s="14">
+        <v>1132440</v>
+      </c>
+      <c r="G14" s="14">
+        <v>97</v>
+      </c>
+      <c r="H14" s="14">
+        <v>344</v>
+      </c>
+      <c r="I14" s="14">
+        <v>343</v>
+      </c>
+      <c r="J14" s="14">
+        <v>344</v>
+      </c>
+      <c r="K14" s="14">
+        <v>344</v>
+      </c>
+      <c r="L14" s="14">
+        <v>373</v>
+      </c>
+      <c r="M14" s="14">
+        <v>4718</v>
+      </c>
+      <c r="N14" s="14">
+        <v>28122</v>
+      </c>
+      <c r="O14" s="14">
+        <v>61190</v>
+      </c>
+      <c r="P14" s="14">
+        <v>368660</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="14">
+        <v>179</v>
+      </c>
+      <c r="C15" s="14">
+        <v>2539</v>
+      </c>
+      <c r="D15" s="14">
+        <v>15372</v>
+      </c>
+      <c r="E15" s="14">
+        <v>32481</v>
+      </c>
+      <c r="F15" s="14">
+        <v>194860</v>
+      </c>
+      <c r="G15" s="14">
+        <v>97</v>
+      </c>
+      <c r="H15" s="14">
+        <v>345</v>
+      </c>
+      <c r="I15" s="14">
+        <v>345</v>
+      </c>
+      <c r="J15" s="14">
+        <v>345</v>
+      </c>
+      <c r="K15" s="14">
+        <v>345</v>
+      </c>
+      <c r="L15" s="14">
+        <v>49</v>
+      </c>
+      <c r="M15" s="14">
+        <v>748</v>
+      </c>
+      <c r="N15" s="14">
+        <v>2748</v>
+      </c>
+      <c r="O15" s="14">
+        <v>5248</v>
+      </c>
+      <c r="P15" s="14">
+        <v>25248</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="B1:P1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="G2:K2"/>
+    <mergeCell ref="L2:P2"/>
+    <mergeCell ref="B9:P9"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="G10:K10"/>
+    <mergeCell ref="L10:P10"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Add the doc with result
And also rename a table with result
</commit_message>
<xml_diff>
--- a/Книга1.xlsx
+++ b/Книга1.xlsx
@@ -91,7 +91,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -234,11 +234,46 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -249,6 +284,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -267,7 +303,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -855,8 +902,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="50624000"/>
-        <c:axId val="50625536"/>
+        <c:axId val="103479552"/>
+        <c:axId val="103374848"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1050,11 +1097,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="50632960"/>
-        <c:axId val="50631424"/>
+        <c:axId val="103377920"/>
+        <c:axId val="103376384"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="50624000"/>
+        <c:axId val="103479552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1064,7 +1111,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50625536"/>
+        <c:crossAx val="103374848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1072,7 +1119,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="50625536"/>
+        <c:axId val="103374848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1083,12 +1130,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50624000"/>
+        <c:crossAx val="103479552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="50631424"/>
+        <c:axId val="103376384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1098,12 +1145,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50632960"/>
+        <c:crossAx val="103377920"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="50632960"/>
+        <c:axId val="103377920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1112,7 +1159,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50631424"/>
+        <c:crossAx val="103376384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1745,11 +1792,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="69360640"/>
-        <c:axId val="69608192"/>
+        <c:axId val="105528320"/>
+        <c:axId val="105538304"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="69360640"/>
+        <c:axId val="105528320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1758,7 +1805,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69608192"/>
+        <c:crossAx val="105538304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1766,7 +1813,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="69608192"/>
+        <c:axId val="105538304"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1778,7 +1825,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69360640"/>
+        <c:crossAx val="105528320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits>
@@ -2400,11 +2447,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="89783296"/>
-        <c:axId val="90047232"/>
+        <c:axId val="105569280"/>
+        <c:axId val="105571072"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="89783296"/>
+        <c:axId val="105569280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2413,7 +2460,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90047232"/>
+        <c:crossAx val="105571072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2421,7 +2468,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="90047232"/>
+        <c:axId val="105571072"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2433,7 +2480,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89783296"/>
+        <c:crossAx val="105569280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2854,52 +2901,52 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="12"/>
-      <c r="P2" s="12"/>
-      <c r="Q2" s="12"/>
-      <c r="R2" s="12"/>
-      <c r="S2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
+      <c r="O2" s="13"/>
+      <c r="P2" s="13"/>
+      <c r="Q2" s="13"/>
+      <c r="R2" s="13"/>
+      <c r="S2" s="14"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="8" t="s">
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="8" t="s">
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="O3" s="9"/>
-      <c r="P3" s="9"/>
-      <c r="Q3" s="9"/>
-      <c r="R3" s="9"/>
-      <c r="S3" s="10"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="10"/>
+      <c r="R3" s="10"/>
+      <c r="S3" s="11"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
@@ -3212,8 +3259,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="P15" sqref="A9:P15"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3223,46 +3270,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="8" t="s">
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="8" t="s">
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="9"/>
-      <c r="N2" s="9"/>
-      <c r="O2" s="9"/>
-      <c r="P2" s="9"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="10"/>
+      <c r="P2" s="10"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
@@ -3316,49 +3363,49 @@
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="14">
+      <c r="B4" s="8">
         <v>2372</v>
       </c>
-      <c r="C4" s="14">
+      <c r="C4" s="8">
         <v>247855</v>
       </c>
-      <c r="D4" s="14">
+      <c r="D4" s="8">
         <v>6301027</v>
       </c>
-      <c r="E4" s="14">
+      <c r="E4" s="8">
         <v>25186062</v>
       </c>
-      <c r="F4" s="14">
+      <c r="F4" s="8">
         <v>625822298</v>
       </c>
-      <c r="G4" s="14">
+      <c r="G4" s="8">
         <v>97</v>
       </c>
-      <c r="H4" s="14">
+      <c r="H4" s="8">
         <v>344</v>
       </c>
-      <c r="I4" s="14">
+      <c r="I4" s="8">
         <v>344</v>
       </c>
-      <c r="J4" s="14">
+      <c r="J4" s="8">
         <v>344</v>
       </c>
-      <c r="K4" s="14">
+      <c r="K4" s="8">
         <v>344</v>
       </c>
-      <c r="L4" s="14">
+      <c r="L4" s="8">
         <v>4851</v>
       </c>
-      <c r="M4" s="14">
+      <c r="M4" s="8">
         <v>498947</v>
       </c>
-      <c r="N4" s="14">
+      <c r="N4" s="8">
         <v>12492947</v>
       </c>
-      <c r="O4" s="14">
+      <c r="O4" s="8">
         <v>49985447</v>
       </c>
-      <c r="P4" s="14">
+      <c r="P4" s="8">
         <v>1249925447</v>
       </c>
     </row>
@@ -3366,49 +3413,49 @@
       <c r="A5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="14">
+      <c r="B5" s="8">
         <v>2501</v>
       </c>
-      <c r="C5" s="14">
+      <c r="C5" s="8">
         <v>250364</v>
       </c>
-      <c r="D5" s="14">
+      <c r="D5" s="8">
         <v>6263870</v>
       </c>
-      <c r="E5" s="14">
+      <c r="E5" s="8">
         <v>24742388</v>
       </c>
-      <c r="F5" s="14">
+      <c r="F5" s="8">
         <v>622195734</v>
       </c>
-      <c r="G5" s="14">
+      <c r="G5" s="8">
         <v>196</v>
       </c>
-      <c r="H5" s="14">
+      <c r="H5" s="8">
         <v>1343</v>
       </c>
-      <c r="I5" s="14">
+      <c r="I5" s="8">
         <v>5343</v>
       </c>
-      <c r="J5" s="14">
+      <c r="J5" s="8">
         <v>10343</v>
       </c>
-      <c r="K5" s="14">
+      <c r="K5" s="8">
         <v>50343</v>
       </c>
-      <c r="L5" s="14">
+      <c r="L5" s="8">
         <v>4852</v>
       </c>
-      <c r="M5" s="14">
+      <c r="M5" s="8">
         <v>499500</v>
       </c>
-      <c r="N5" s="14">
+      <c r="N5" s="8">
         <v>12497500</v>
       </c>
-      <c r="O5" s="14">
+      <c r="O5" s="8">
         <v>49995000</v>
       </c>
-      <c r="P5" s="14">
+      <c r="P5" s="8">
         <v>1249975000</v>
       </c>
     </row>
@@ -3416,49 +3463,49 @@
       <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="14">
+      <c r="B6" s="8">
         <v>940</v>
       </c>
-      <c r="C6" s="14">
+      <c r="C6" s="8">
         <v>14852</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6" s="8">
         <v>112646</v>
       </c>
-      <c r="E6" s="14">
+      <c r="E6" s="8">
         <v>257359</v>
       </c>
-      <c r="F6" s="14">
+      <c r="F6" s="8">
         <v>1806986</v>
       </c>
-      <c r="G6" s="14">
+      <c r="G6" s="8">
         <v>595</v>
       </c>
-      <c r="H6" s="14">
+      <c r="H6" s="8">
         <v>8434</v>
       </c>
-      <c r="I6" s="14">
+      <c r="I6" s="8">
         <v>55342</v>
       </c>
-      <c r="J6" s="14">
+      <c r="J6" s="8">
         <v>120342</v>
       </c>
-      <c r="K6" s="14">
+      <c r="K6" s="8">
         <v>700343</v>
       </c>
-      <c r="L6" s="14">
+      <c r="L6" s="8">
         <v>744</v>
       </c>
-      <c r="M6" s="14">
+      <c r="M6" s="8">
         <v>11735</v>
       </c>
-      <c r="N6" s="14">
+      <c r="N6" s="8">
         <v>78143</v>
       </c>
-      <c r="O6" s="14">
+      <c r="O6" s="8">
         <v>171212</v>
       </c>
-      <c r="P6" s="14">
+      <c r="P6" s="8">
         <v>1018691</v>
       </c>
     </row>
@@ -3466,93 +3513,93 @@
       <c r="A7" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="14">
+      <c r="B7" s="8">
         <v>532</v>
       </c>
-      <c r="C7" s="14">
+      <c r="C7" s="8">
         <v>8213</v>
       </c>
-      <c r="D7" s="14">
+      <c r="D7" s="8">
         <v>48893</v>
       </c>
-      <c r="E7" s="14">
+      <c r="E7" s="8">
         <v>116593</v>
       </c>
-      <c r="F7" s="14">
+      <c r="F7" s="8">
         <v>645555</v>
       </c>
-      <c r="G7" s="14">
+      <c r="G7" s="8">
         <v>578</v>
       </c>
-      <c r="H7" s="14">
+      <c r="H7" s="8">
         <v>9631</v>
       </c>
-      <c r="I7" s="14">
+      <c r="I7" s="8">
         <v>61464</v>
       </c>
-      <c r="J7" s="14">
+      <c r="J7" s="8">
         <v>133272</v>
       </c>
-      <c r="K7" s="14">
+      <c r="K7" s="8">
         <v>784119</v>
       </c>
-      <c r="L7" s="14">
+      <c r="L7" s="8">
         <v>575</v>
       </c>
-      <c r="M7" s="14">
+      <c r="M7" s="8">
         <v>8730</v>
       </c>
-      <c r="N7" s="14">
+      <c r="N7" s="8">
         <v>56563</v>
       </c>
-      <c r="O7" s="14">
+      <c r="O7" s="8">
         <v>123371</v>
       </c>
-      <c r="P7" s="14">
+      <c r="P7" s="8">
         <v>754217</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="11" t="s">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B9" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="12"/>
-      <c r="L9" s="12"/>
-      <c r="M9" s="12"/>
-      <c r="N9" s="12"/>
-      <c r="O9" s="12"/>
-      <c r="P9" s="12"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="18"/>
+      <c r="M9" s="18"/>
+      <c r="N9" s="18"/>
+      <c r="O9" s="18"/>
+      <c r="P9" s="18"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="8" t="s">
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="8" t="s">
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="M10" s="9"/>
-      <c r="N10" s="9"/>
-      <c r="O10" s="9"/>
-      <c r="P10" s="9"/>
+      <c r="M10" s="17"/>
+      <c r="N10" s="17"/>
+      <c r="O10" s="17"/>
+      <c r="P10" s="17"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
@@ -3606,49 +3653,49 @@
       <c r="A12" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="14">
+      <c r="B12" s="8">
         <v>2372</v>
       </c>
-      <c r="C12" s="14">
+      <c r="C12" s="8">
         <v>247855</v>
       </c>
-      <c r="D12" s="14">
+      <c r="D12" s="8">
         <v>6301027</v>
       </c>
-      <c r="E12" s="14">
+      <c r="E12" s="8">
         <v>25186062</v>
       </c>
-      <c r="F12" s="14">
+      <c r="F12" s="8">
         <v>625822298</v>
       </c>
-      <c r="G12" s="14">
+      <c r="G12" s="8">
         <v>97</v>
       </c>
-      <c r="H12" s="14">
+      <c r="H12" s="8">
         <v>344</v>
       </c>
-      <c r="I12" s="14">
+      <c r="I12" s="8">
         <v>344</v>
       </c>
-      <c r="J12" s="14">
+      <c r="J12" s="8">
         <v>344</v>
       </c>
-      <c r="K12" s="14">
+      <c r="K12" s="8">
         <v>344</v>
       </c>
-      <c r="L12" s="14">
+      <c r="L12" s="8">
         <v>4851</v>
       </c>
-      <c r="M12" s="14">
+      <c r="M12" s="8">
         <v>498947</v>
       </c>
-      <c r="N12" s="14">
+      <c r="N12" s="8">
         <v>12492947</v>
       </c>
-      <c r="O12" s="14">
+      <c r="O12" s="8">
         <v>49985447</v>
       </c>
-      <c r="P12" s="14">
+      <c r="P12" s="8">
         <v>1249925447</v>
       </c>
     </row>
@@ -3656,49 +3703,49 @@
       <c r="A13" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B13" s="14">
+      <c r="B13" s="8">
         <v>2405</v>
       </c>
-      <c r="C13" s="14">
+      <c r="C13" s="8">
         <v>249373</v>
       </c>
-      <c r="D13" s="14">
+      <c r="D13" s="8">
         <v>6258876</v>
       </c>
-      <c r="E13" s="14">
+      <c r="E13" s="8">
         <v>24732396</v>
       </c>
-      <c r="F13" s="14">
+      <c r="F13" s="8">
         <v>622145750</v>
       </c>
-      <c r="G13" s="14">
+      <c r="G13" s="8">
         <v>97</v>
       </c>
-      <c r="H13" s="14">
+      <c r="H13" s="8">
         <v>344</v>
       </c>
-      <c r="I13" s="14">
+      <c r="I13" s="8">
         <v>344</v>
       </c>
-      <c r="J13" s="14">
+      <c r="J13" s="8">
         <v>344</v>
       </c>
-      <c r="K13" s="14">
+      <c r="K13" s="8">
         <v>344</v>
       </c>
-      <c r="L13" s="14">
+      <c r="L13" s="8">
         <v>4851</v>
       </c>
-      <c r="M13" s="14">
+      <c r="M13" s="8">
         <v>498947</v>
       </c>
-      <c r="N13" s="14">
+      <c r="N13" s="8">
         <v>12492947</v>
       </c>
-      <c r="O13" s="14">
+      <c r="O13" s="8">
         <v>49985447</v>
       </c>
-      <c r="P13" s="14">
+      <c r="P13" s="8">
         <v>1249925447</v>
       </c>
     </row>
@@ -3706,49 +3753,49 @@
       <c r="A14" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="14">
+      <c r="B14" s="8">
         <v>487</v>
       </c>
-      <c r="C14" s="14">
+      <c r="C14" s="8">
         <v>7369</v>
       </c>
-      <c r="D14" s="14">
+      <c r="D14" s="8">
         <v>60182</v>
       </c>
-      <c r="E14" s="14">
+      <c r="E14" s="8">
         <v>1422475</v>
       </c>
-      <c r="F14" s="14">
+      <c r="F14" s="8">
         <v>1132440</v>
       </c>
-      <c r="G14" s="14">
+      <c r="G14" s="8">
         <v>97</v>
       </c>
-      <c r="H14" s="14">
+      <c r="H14" s="8">
         <v>344</v>
       </c>
-      <c r="I14" s="14">
+      <c r="I14" s="8">
         <v>343</v>
       </c>
-      <c r="J14" s="14">
+      <c r="J14" s="8">
         <v>344</v>
       </c>
-      <c r="K14" s="14">
+      <c r="K14" s="8">
         <v>344</v>
       </c>
-      <c r="L14" s="14">
+      <c r="L14" s="8">
         <v>373</v>
       </c>
-      <c r="M14" s="14">
+      <c r="M14" s="8">
         <v>4718</v>
       </c>
-      <c r="N14" s="14">
+      <c r="N14" s="8">
         <v>28122</v>
       </c>
-      <c r="O14" s="14">
+      <c r="O14" s="8">
         <v>61190</v>
       </c>
-      <c r="P14" s="14">
+      <c r="P14" s="8">
         <v>368660</v>
       </c>
     </row>
@@ -3756,62 +3803,62 @@
       <c r="A15" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="14">
+      <c r="B15" s="8">
         <v>179</v>
       </c>
-      <c r="C15" s="14">
+      <c r="C15" s="8">
         <v>2539</v>
       </c>
-      <c r="D15" s="14">
+      <c r="D15" s="8">
         <v>15372</v>
       </c>
-      <c r="E15" s="14">
+      <c r="E15" s="8">
         <v>32481</v>
       </c>
-      <c r="F15" s="14">
+      <c r="F15" s="8">
         <v>194860</v>
       </c>
-      <c r="G15" s="14">
+      <c r="G15" s="8">
         <v>97</v>
       </c>
-      <c r="H15" s="14">
+      <c r="H15" s="8">
         <v>345</v>
       </c>
-      <c r="I15" s="14">
+      <c r="I15" s="8">
         <v>345</v>
       </c>
-      <c r="J15" s="14">
+      <c r="J15" s="8">
         <v>345</v>
       </c>
-      <c r="K15" s="14">
+      <c r="K15" s="8">
         <v>345</v>
       </c>
-      <c r="L15" s="14">
+      <c r="L15" s="8">
         <v>49</v>
       </c>
-      <c r="M15" s="14">
+      <c r="M15" s="8">
         <v>748</v>
       </c>
-      <c r="N15" s="14">
+      <c r="N15" s="8">
         <v>2748</v>
       </c>
-      <c r="O15" s="14">
+      <c r="O15" s="8">
         <v>5248</v>
       </c>
-      <c r="P15" s="14">
+      <c r="P15" s="8">
         <v>25248</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="G10:K10"/>
+    <mergeCell ref="L10:P10"/>
     <mergeCell ref="B1:P1"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="G2:K2"/>
     <mergeCell ref="L2:P2"/>
     <mergeCell ref="B9:P9"/>
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="G10:K10"/>
-    <mergeCell ref="L10:P10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>